<commit_message>
bootstrapped rifdid with dropped states
</commit_message>
<xml_diff>
--- a/linreg/rifdid_coefs-sltt.xlsx
+++ b/linreg/rifdid_coefs-sltt.xlsx
@@ -582,16 +582,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.09966750589946724</v>
+        <v>-0.09894051921768969</v>
       </c>
       <c r="C2">
-        <v>0.0051871731743450226</v>
+        <v>0.004514657706317109</v>
       </c>
       <c r="D2">
-        <v>-0.10983419026343223</v>
+        <v>-0.10778909637368989</v>
       </c>
       <c r="E2">
-        <v>-0.089500821535502248</v>
+        <v>-0.090091942061689495</v>
       </c>
     </row>
     <row r="3">
@@ -599,16 +599,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>-0.041029700851240303</v>
+        <v>-0.043533415441654164</v>
       </c>
       <c r="C3">
-        <v>0.009224613156953318</v>
+        <v>0.0090782012124654334</v>
       </c>
       <c r="D3">
-        <v>-0.059109631324790558</v>
+        <v>-0.061326384275990117</v>
       </c>
       <c r="E3">
-        <v>-0.022949770377690047</v>
+        <v>-0.025740446607318213</v>
       </c>
     </row>
     <row r="4">
@@ -616,16 +616,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-0.11478106127942626</v>
+        <v>-0.11607737415090387</v>
       </c>
       <c r="C4">
-        <v>0.007946079577654681</v>
+        <v>0.0084440974305450712</v>
       </c>
       <c r="D4">
-        <v>-0.13035510908575654</v>
+        <v>-0.13262752091450281</v>
       </c>
       <c r="E4">
-        <v>-0.09920701347309599</v>
+        <v>-0.099527227387304934</v>
       </c>
     </row>
     <row r="5">
@@ -633,16 +633,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-0.031061756489655794</v>
+        <v>-0.030933566121955063</v>
       </c>
       <c r="C5">
-        <v>0.0029214773428446542</v>
+        <v>0.0026597104253623552</v>
       </c>
       <c r="D5">
-        <v>-0.03678775341294304</v>
+        <v>-0.036146508982317228</v>
       </c>
       <c r="E5">
-        <v>-0.025335759566368545</v>
+        <v>-0.025720623261592898</v>
       </c>
     </row>
     <row r="6">
@@ -650,16 +650,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-0.043193825420974115</v>
+        <v>-0.042416564243250722</v>
       </c>
       <c r="C6">
-        <v>0.0081878453874787618</v>
+        <v>0.0078866387341627302</v>
       </c>
       <c r="D6">
-        <v>-0.059241725847750781</v>
+        <v>-0.057874110557116137</v>
       </c>
       <c r="E6">
-        <v>-0.027145924994197452</v>
+        <v>-0.026959017929385303</v>
       </c>
     </row>
     <row r="7">
@@ -667,16 +667,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>-0.079676915233941589</v>
+        <v>-0.07977017011835015</v>
       </c>
       <c r="C7">
-        <v>0.0043933710236810086</v>
+        <v>0.0046389518947940528</v>
       </c>
       <c r="D7">
-        <v>-0.088287774060579582</v>
+        <v>-0.088862359602186761</v>
       </c>
       <c r="E7">
-        <v>-0.071066056407303596</v>
+        <v>-0.07067798063451354</v>
       </c>
     </row>
     <row r="8">
@@ -684,16 +684,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-0.10484200599848044</v>
+        <v>-0.10464121954759192</v>
       </c>
       <c r="C8">
-        <v>0.0058051350946869227</v>
+        <v>0.0056256901752176547</v>
       </c>
       <c r="D8">
-        <v>-0.11621987771931241</v>
+        <v>-0.11566738584075847</v>
       </c>
       <c r="E8">
-        <v>-0.093464134277648464</v>
+        <v>-0.093615053254425373</v>
       </c>
     </row>
     <row r="9">
@@ -701,16 +701,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>-0.040311058800035056</v>
+        <v>-0.041315305200016916</v>
       </c>
       <c r="C9">
-        <v>0.010250296810096366</v>
+        <v>0.010078463130816668</v>
       </c>
       <c r="D9">
-        <v>-0.060401299647740853</v>
+        <v>-0.061068758909478091</v>
       </c>
       <c r="E9">
-        <v>-0.020220817952329259</v>
+        <v>-0.021561851490555738</v>
       </c>
     </row>
     <row r="10">
@@ -718,16 +718,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>-0.086321543221335131</v>
+        <v>-0.086539793603786566</v>
       </c>
       <c r="C10">
-        <v>0.0076043008634790318</v>
+        <v>0.0087496405902062202</v>
       </c>
       <c r="D10">
-        <v>-0.10122572001309718</v>
+        <v>-0.10368879917434681</v>
       </c>
       <c r="E10">
-        <v>-0.071417366429573081</v>
+        <v>-0.069390788033226319</v>
       </c>
     </row>
     <row r="11">
@@ -735,16 +735,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.035711457716555955</v>
+        <v>-0.035665816068694393</v>
       </c>
       <c r="C11">
-        <v>0.0033217401245571932</v>
+        <v>0.0033477031822628346</v>
       </c>
       <c r="D11">
-        <v>-0.042221957431516015</v>
+        <v>-0.042227202884721877</v>
       </c>
       <c r="E11">
-        <v>-0.029200958001595896</v>
+        <v>-0.029104429252666913</v>
       </c>
     </row>
     <row r="12">
@@ -752,16 +752,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>-0.028283525667819241</v>
+        <v>-0.028272901593313287</v>
       </c>
       <c r="C12">
-        <v>0.0066108253822414666</v>
+        <v>0.0065260662674304455</v>
       </c>
       <c r="D12">
-        <v>-0.041240522649174383</v>
+        <v>-0.041063774271187965</v>
       </c>
       <c r="E12">
-        <v>-0.0153265286864641</v>
+        <v>-0.01548202891543861</v>
       </c>
     </row>
     <row r="13">
@@ -769,16 +769,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>-0.067475187204618647</v>
+        <v>-0.067265343882454406</v>
       </c>
       <c r="C13">
-        <v>0.0046321979750882118</v>
+        <v>0.0043034942704115427</v>
       </c>
       <c r="D13">
-        <v>-0.076554140544013494</v>
+        <v>-0.075700049419772014</v>
       </c>
       <c r="E13">
-        <v>-0.058396233865223801</v>
+        <v>-0.058830638345136799</v>
       </c>
     </row>
     <row r="14">
@@ -786,16 +786,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-0.22138637261767674</v>
+        <v>-0.22237912079548788</v>
       </c>
       <c r="C14">
-        <v>0.0098200686463172093</v>
+        <v>0.010932886883365049</v>
       </c>
       <c r="D14">
-        <v>-0.2406334797401033</v>
+        <v>-0.24380733074169428</v>
       </c>
       <c r="E14">
-        <v>-0.20213926549525019</v>
+        <v>-0.20095091084928149</v>
       </c>
     </row>
     <row r="15">
@@ -803,16 +803,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>-0.049114955930223525</v>
+        <v>-0.050190966664693908</v>
       </c>
       <c r="C15">
-        <v>0.026397465681400521</v>
+        <v>0.023571704593621508</v>
       </c>
       <c r="D15">
-        <v>-0.10085337732313675</v>
+        <v>-0.096390972226867433</v>
       </c>
       <c r="E15">
-        <v>0.0026234654626896975</v>
+        <v>-0.0039909611025203823</v>
       </c>
     </row>
     <row r="16">
@@ -820,16 +820,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>-0.064237187362483059</v>
+        <v>-0.060893894220289874</v>
       </c>
       <c r="C16">
-        <v>0.018880125586225961</v>
+        <v>0.018278189287848547</v>
       </c>
       <c r="D16">
-        <v>-0.10124179626399393</v>
+        <v>-0.096718730027606586</v>
       </c>
       <c r="E16">
-        <v>-0.027232578460972184</v>
+        <v>-0.025069058412973168</v>
       </c>
     </row>
     <row r="17">
@@ -837,16 +837,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>-0.056847681417502662</v>
+        <v>-0.055840382178051977</v>
       </c>
       <c r="C17">
-        <v>0.0081300779136355503</v>
+        <v>0.0079506800999507698</v>
       </c>
       <c r="D17">
-        <v>-0.072782468928401373</v>
+        <v>-0.071423558943240928</v>
       </c>
       <c r="E17">
-        <v>-0.040912893906603957</v>
+        <v>-0.040257205412863026</v>
       </c>
     </row>
     <row r="18">
@@ -854,16 +854,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.03959665511174789</v>
+        <v>0.042482134741117075</v>
       </c>
       <c r="C18">
-        <v>0.028498381319269309</v>
+        <v>0.027933214867877393</v>
       </c>
       <c r="D18">
-        <v>-0.016259593198676155</v>
+        <v>-0.012266417512775372</v>
       </c>
       <c r="E18">
-        <v>0.095452903422171942</v>
+        <v>0.09723068699500953</v>
       </c>
     </row>
     <row r="19">
@@ -871,16 +871,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>-0.092243562551230215</v>
+        <v>-0.093666094258727572</v>
       </c>
       <c r="C19">
-        <v>0.016204183425653752</v>
+        <v>0.01565513785022505</v>
       </c>
       <c r="D19">
-        <v>-0.12400343280319372</v>
+        <v>-0.1243498568220041</v>
       </c>
       <c r="E19">
-        <v>-0.060483692299266714</v>
+        <v>-0.062982331695451046</v>
       </c>
     </row>
     <row r="20">
@@ -888,16 +888,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>-0.15334035953455341</v>
+        <v>-0.15371635365170302</v>
       </c>
       <c r="C20">
-        <v>0.0044959052604388828</v>
+        <v>0.0048186284221387954</v>
       </c>
       <c r="D20">
-        <v>-0.16215218211630933</v>
+        <v>-0.16316070318006917</v>
       </c>
       <c r="E20">
-        <v>-0.14452853695279749</v>
+        <v>-0.14427200412333688</v>
       </c>
     </row>
     <row r="21">
@@ -905,16 +905,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>-0.024915921447227329</v>
+        <v>-0.024975055973752484</v>
       </c>
       <c r="C21">
-        <v>0.0080897341161169038</v>
+        <v>0.0091685468373012176</v>
       </c>
       <c r="D21">
-        <v>-0.040771527300861643</v>
+        <v>-0.042945099192032959</v>
       </c>
       <c r="E21">
-        <v>-0.0090603155935930109</v>
+        <v>-0.0070050127554720128</v>
       </c>
     </row>
     <row r="22">
@@ -922,16 +922,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>-0.11707349300476344</v>
+        <v>-0.11728900913158156</v>
       </c>
       <c r="C22">
-        <v>0.0064268017758319406</v>
+        <v>0.0068605287932954461</v>
       </c>
       <c r="D22">
-        <v>-0.12966980759241037</v>
+        <v>-0.13073541466383118</v>
       </c>
       <c r="E22">
-        <v>-0.10447717841711651</v>
+        <v>-0.10384260359933195</v>
       </c>
     </row>
     <row r="23">
@@ -939,16 +939,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>-0.047843545660824383</v>
+        <v>-0.047961391987491747</v>
       </c>
       <c r="C23">
-        <v>0.0027653378310304763</v>
+        <v>0.00287092887707545</v>
       </c>
       <c r="D23">
-        <v>-0.053263514414342905</v>
+        <v>-0.053588315899826711</v>
       </c>
       <c r="E23">
-        <v>-0.04242357690730586</v>
+        <v>-0.042334468075156784</v>
       </c>
     </row>
     <row r="24">
@@ -956,16 +956,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>-0.073117036191376036</v>
+        <v>-0.073282962405392144</v>
       </c>
       <c r="C24">
-        <v>0.0077056715567641746</v>
+        <v>0.0067675556385943837</v>
       </c>
       <c r="D24">
-        <v>-0.088219892194678573</v>
+        <v>-0.086547143540264354</v>
       </c>
       <c r="E24">
-        <v>-0.0580141801880735</v>
+        <v>-0.060018781270519933</v>
       </c>
     </row>
     <row r="25">
@@ -973,16 +973,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>-0.0940270797513683</v>
+        <v>-0.094185791471637456</v>
       </c>
       <c r="C25">
-        <v>0.0042304808598042695</v>
+        <v>0.0045119619268859943</v>
       </c>
       <c r="D25">
-        <v>-0.1023186793581885</v>
+        <v>-0.10302908489512427</v>
       </c>
       <c r="E25">
-        <v>-0.085735480144548099</v>
+        <v>-0.085342498048150639</v>
       </c>
     </row>
     <row r="26">
@@ -990,16 +990,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>-0.16164730108268732</v>
+        <v>-0.16195412493578826</v>
       </c>
       <c r="C26">
-        <v>0.005715043589491633</v>
+        <v>0.0053779741465521651</v>
       </c>
       <c r="D26">
-        <v>-0.17284859644956213</v>
+        <v>-0.17249477602273519</v>
       </c>
       <c r="E26">
-        <v>-0.15044600571581251</v>
+        <v>-0.15141347384884132</v>
       </c>
     </row>
     <row r="27">
@@ -1007,16 +1007,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>-0.021022013504616549</v>
+        <v>-0.021024122318323662</v>
       </c>
       <c r="C27">
-        <v>0.010221459813432848</v>
+        <v>0.009456819325115582</v>
       </c>
       <c r="D27">
-        <v>-0.041055734797910623</v>
+        <v>-0.039559174771531536</v>
       </c>
       <c r="E27">
-        <v>-0.0009882922113224786</v>
+        <v>-0.0024890698651157915</v>
       </c>
     </row>
     <row r="28">
@@ -1024,16 +1024,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>-0.079120006348139871</v>
+        <v>-0.079259547911632186</v>
       </c>
       <c r="C28">
-        <v>0.0070803052493718975</v>
+        <v>0.0069920616867580132</v>
       </c>
       <c r="D28">
-        <v>-0.09299716916307886</v>
+        <v>-0.09296375708225002</v>
       </c>
       <c r="E28">
-        <v>-0.065242843533200881</v>
+        <v>-0.065555338741014352</v>
       </c>
     </row>
     <row r="29">
@@ -1041,16 +1041,16 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>-0.057420294977881876</v>
+        <v>-0.057539015430956006</v>
       </c>
       <c r="C29">
-        <v>0.0031233743217507254</v>
+        <v>0.0034102257500477659</v>
       </c>
       <c r="D29">
-        <v>-0.063542004343746974</v>
+        <v>-0.064222944398910756</v>
       </c>
       <c r="E29">
-        <v>-0.051298585612016778</v>
+        <v>-0.050855086463001263</v>
       </c>
     </row>
     <row r="30">
@@ -1058,16 +1058,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>-0.061340953745580871</v>
+        <v>-0.061424857223817388</v>
       </c>
       <c r="C30">
-        <v>0.0071670286661993992</v>
+        <v>0.0070792417432372383</v>
       </c>
       <c r="D30">
-        <v>-0.075388090589141726</v>
+        <v>-0.075299935422999675</v>
       </c>
       <c r="E30">
-        <v>-0.047293816902020017</v>
+        <v>-0.0475497790246351</v>
       </c>
     </row>
     <row r="31">
@@ -1075,16 +1075,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>-0.075119690272628742</v>
+        <v>-0.075079613051327293</v>
       </c>
       <c r="C31">
-        <v>0.0044480553395300319</v>
+        <v>0.004711179840784176</v>
       </c>
       <c r="D31">
-        <v>-0.083837730195754051</v>
+        <v>-0.084313368737624808</v>
       </c>
       <c r="E31">
-        <v>-0.066401650349503433</v>
+        <v>-0.065845857365029778</v>
       </c>
     </row>
     <row r="32">
@@ -1092,16 +1092,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>-0.17802183957759937</v>
+        <v>-0.17884425021103528</v>
       </c>
       <c r="C32">
-        <v>0.0067454293161856218</v>
+        <v>0.0067468441590282152</v>
       </c>
       <c r="D32">
-        <v>-0.19124272481897403</v>
+        <v>-0.19206791150528757</v>
       </c>
       <c r="E32">
-        <v>-0.16480095433622471</v>
+        <v>-0.165620588916783</v>
       </c>
     </row>
     <row r="33">
@@ -1109,16 +1109,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>-0.044964411984423643</v>
+        <v>-0.044107527186619179</v>
       </c>
       <c r="C33">
-        <v>0.018065166707769302</v>
+        <v>0.021242536826180325</v>
       </c>
       <c r="D33">
-        <v>-0.0803717203579071</v>
+        <v>-0.085742416832647356</v>
       </c>
       <c r="E33">
-        <v>-0.0095571036109401847</v>
+        <v>-0.0024726375405910023</v>
       </c>
     </row>
     <row r="34">
@@ -1126,16 +1126,16 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>-0.058319072371150776</v>
+        <v>-0.059048915991676103</v>
       </c>
       <c r="C34">
-        <v>0.013646650726491997</v>
+        <v>0.012892191780831654</v>
       </c>
       <c r="D34">
-        <v>-0.085066191750365686</v>
+        <v>-0.084317319030470531</v>
       </c>
       <c r="E34">
-        <v>-0.031571952991935867</v>
+        <v>-0.033780512952881675</v>
       </c>
     </row>
     <row r="35">
@@ -1143,16 +1143,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>-0.04829739826132752</v>
+        <v>-0.048562589185836974</v>
       </c>
       <c r="C35">
-        <v>0.0066198675751617808</v>
+        <v>0.0061962499578786202</v>
       </c>
       <c r="D35">
-        <v>-0.061272204195668277</v>
+        <v>-0.060707117347083839</v>
       </c>
       <c r="E35">
-        <v>-0.035322592326986764</v>
+        <v>-0.036418061024590109</v>
       </c>
     </row>
     <row r="36">
@@ -1160,16 +1160,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>0.0009635710774647747</v>
+        <v>0.0018021788135040085</v>
       </c>
       <c r="C36">
-        <v>0.02191763936917052</v>
+        <v>0.02111442115140863</v>
       </c>
       <c r="D36">
-        <v>-0.04199455672872543</v>
+        <v>-0.03958167174527806</v>
       </c>
       <c r="E36">
-        <v>0.043921698883654978</v>
+        <v>0.043186029372286078</v>
       </c>
     </row>
     <row r="37">
@@ -1177,16 +1177,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>-0.080404058333459039</v>
+        <v>-0.080981693029874721</v>
       </c>
       <c r="C37">
-        <v>0.011107348425762132</v>
+        <v>0.011394714186114523</v>
       </c>
       <c r="D37">
-        <v>-0.1021742355512181</v>
+        <v>-0.10331510892873956</v>
       </c>
       <c r="E37">
-        <v>-0.058633881115699976</v>
+        <v>-0.058648277131009882</v>
       </c>
     </row>
     <row r="38">
@@ -1194,16 +1194,16 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>-0.16992914568263587</v>
+        <v>-0.17077972922230547</v>
       </c>
       <c r="C38">
-        <v>0.0037854115319419829</v>
+        <v>0.0042443717788707156</v>
       </c>
       <c r="D38">
-        <v>-0.1773484245344214</v>
+        <v>-0.17909855505743721</v>
       </c>
       <c r="E38">
-        <v>-0.16250986683085034</v>
+        <v>-0.16246090338717373</v>
       </c>
     </row>
     <row r="39">
@@ -1211,16 +1211,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>-0.01515627951917595</v>
+        <v>-0.016555268981886015</v>
       </c>
       <c r="C39">
-        <v>0.0082048809046865491</v>
+        <v>0.0086608009149261034</v>
       </c>
       <c r="D39">
-        <v>-0.031237569192410067</v>
+        <v>-0.033530147281352347</v>
       </c>
       <c r="E39">
-        <v>0.00092501015405816595</v>
+        <v>0.00041960931758031755</v>
       </c>
     </row>
     <row r="40">
@@ -1228,16 +1228,16 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>-0.088287019894326468</v>
+        <v>-0.088379158186197085</v>
       </c>
       <c r="C40">
-        <v>0.0054989241750990443</v>
+        <v>0.0053513528358412376</v>
       </c>
       <c r="D40">
-        <v>-0.099064725698734604</v>
+        <v>-0.098867629635685905</v>
       </c>
       <c r="E40">
-        <v>-0.077509314089918332</v>
+        <v>-0.077890686736708264</v>
       </c>
     </row>
     <row r="41">
@@ -1245,16 +1245,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>-0.062913723516511852</v>
+        <v>-0.063005120857151792</v>
       </c>
       <c r="C41">
-        <v>0.0029271913355892036</v>
+        <v>0.0028719188310663687</v>
       </c>
       <c r="D41">
-        <v>-0.068650919672596539</v>
+        <v>-0.068633985045969431</v>
       </c>
       <c r="E41">
-        <v>-0.057176527360427158</v>
+        <v>-0.057376256668334159</v>
       </c>
     </row>
     <row r="42">
@@ -1262,16 +1262,16 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>-0.047835364204096315</v>
+        <v>-0.048199204343522109</v>
       </c>
       <c r="C42">
-        <v>0.0076665417285096248</v>
+        <v>0.0079729666828337546</v>
       </c>
       <c r="D42">
-        <v>-0.062861527065573505</v>
+        <v>-0.063825950529442399</v>
       </c>
       <c r="E42">
-        <v>-0.032809201342619124</v>
+        <v>-0.032572458157601819</v>
       </c>
     </row>
     <row r="43">
@@ -1279,16 +1279,16 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>-0.088207534561916837</v>
+        <v>-0.088553136146247449</v>
       </c>
       <c r="C43">
-        <v>0.0042028065419818803</v>
+        <v>0.0045064926206093408</v>
       </c>
       <c r="D43">
-        <v>-0.096444893440465362</v>
+        <v>-0.09738570991362655</v>
       </c>
       <c r="E43">
-        <v>-0.079970175683368311</v>
+        <v>-0.079720562378868348</v>
       </c>
     </row>
     <row r="44">
@@ -1296,16 +1296,16 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>-0.18253326135599404</v>
+        <v>-0.18392056238515603</v>
       </c>
       <c r="C44">
-        <v>0.0044691892234699025</v>
+        <v>0.0047912073137086073</v>
       </c>
       <c r="D44">
-        <v>-0.19129272359956956</v>
+        <v>-0.19331116992673522</v>
       </c>
       <c r="E44">
-        <v>-0.17377379911241853</v>
+        <v>-0.17452995484357683</v>
       </c>
     </row>
     <row r="45">
@@ -1313,16 +1313,16 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>-0.0139521592400681</v>
+        <v>-0.018203832247304846</v>
       </c>
       <c r="C45">
-        <v>0.0080272977075667475</v>
+        <v>0.0084221537673135078</v>
       </c>
       <c r="D45">
-        <v>-0.029685395778390002</v>
+        <v>-0.034710974498775346</v>
       </c>
       <c r="E45">
-        <v>0.0017810772982538026</v>
+        <v>-0.0016966899958343468</v>
       </c>
     </row>
     <row r="46">
@@ -1330,16 +1330,16 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>-0.06246124660326708</v>
+        <v>-0.061859200075038069</v>
       </c>
       <c r="C46">
-        <v>0.0057450113842309834</v>
+        <v>0.0067533460980290609</v>
       </c>
       <c r="D46">
-        <v>-0.073721277851174633</v>
+        <v>-0.075095534603413491</v>
       </c>
       <c r="E46">
-        <v>-0.051201215355359535</v>
+        <v>-0.048622865546662647</v>
       </c>
     </row>
     <row r="47">
@@ -1347,16 +1347,16 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>-0.079835604191876491</v>
+        <v>-0.080024080192772892</v>
       </c>
       <c r="C47">
-        <v>0.0033806413270745157</v>
+        <v>0.0035248897303533952</v>
       </c>
       <c r="D47">
-        <v>-0.086461548296770857</v>
+        <v>-0.086932746745779027</v>
       </c>
       <c r="E47">
-        <v>-0.073209660086982126</v>
+        <v>-0.073115413639766758</v>
       </c>
     </row>
     <row r="48">
@@ -1364,16 +1364,16 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>-0.069777522386801044</v>
+        <v>-0.069775801888453171</v>
       </c>
       <c r="C48">
-        <v>0.0078010443242021782</v>
+        <v>0.0085922174348576352</v>
       </c>
       <c r="D48">
-        <v>-0.085067308747159232</v>
+        <v>-0.08661626208702107</v>
       </c>
       <c r="E48">
-        <v>-0.054487736026442857</v>
+        <v>-0.052935341689885271</v>
       </c>
     </row>
     <row r="49">
@@ -1381,16 +1381,16 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>-0.06897116219040178</v>
+        <v>-0.069210112341567251</v>
       </c>
       <c r="C49">
-        <v>0.004765654230233788</v>
+        <v>0.0047979448676714592</v>
       </c>
       <c r="D49">
-        <v>-0.078311685333123951</v>
+        <v>-0.078613924592773748</v>
       </c>
       <c r="E49">
-        <v>-0.059630639047679609</v>
+        <v>-0.059806300090360753</v>
       </c>
     </row>
     <row r="50">
@@ -1398,16 +1398,16 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>-0.15567390608313189</v>
+        <v>-0.15635913994518336</v>
       </c>
       <c r="C50">
-        <v>0.0057160706751824926</v>
+        <v>0.005973922551482558</v>
       </c>
       <c r="D50">
-        <v>-0.16687727222720239</v>
+        <v>-0.16806789244589015</v>
       </c>
       <c r="E50">
-        <v>-0.14447053993906139</v>
+        <v>-0.14465038744447656</v>
       </c>
     </row>
     <row r="51">
@@ -1415,16 +1415,16 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>-0.036703837007708934</v>
+        <v>-0.035642511590798072</v>
       </c>
       <c r="C51">
-        <v>0.015645647444940583</v>
+        <v>0.017933421877137132</v>
       </c>
       <c r="D51">
-        <v>-0.067368943660036054</v>
+        <v>-0.070791611104659202</v>
       </c>
       <c r="E51">
-        <v>-0.0060387303553818134</v>
+        <v>-0.0004934120769369485</v>
       </c>
     </row>
     <row r="52">
@@ -1432,16 +1432,16 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>-0.036536496075590903</v>
+        <v>-0.036235974858454284</v>
       </c>
       <c r="C52">
-        <v>0.010284176103703829</v>
+        <v>0.010945260625626915</v>
       </c>
       <c r="D52">
-        <v>-0.056693243066165161</v>
+        <v>-0.057688437058419098</v>
       </c>
       <c r="E52">
-        <v>-0.016379749085016649</v>
+        <v>-0.01478351265848947</v>
       </c>
     </row>
     <row r="53">
@@ -1449,16 +1449,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>-0.04876957860162541</v>
+        <v>-0.048935438769268508</v>
       </c>
       <c r="C53">
-        <v>0.0048544769952561032</v>
+        <v>0.0052227131314060409</v>
       </c>
       <c r="D53">
-        <v>-0.05828425487135884</v>
+        <v>-0.059171853880609457</v>
       </c>
       <c r="E53">
-        <v>-0.03925490233189198</v>
+        <v>-0.038699023657927559</v>
       </c>
     </row>
     <row r="54">
@@ -1466,16 +1466,16 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>-0.0083608857364644608</v>
+        <v>-0.0081101470447616977</v>
       </c>
       <c r="C54">
-        <v>0.019551057156132333</v>
+        <v>0.019239845078002332</v>
       </c>
       <c r="D54">
-        <v>-0.046680560493073425</v>
+        <v>-0.045819865335052036</v>
       </c>
       <c r="E54">
-        <v>0.0299587890201445</v>
+        <v>0.029599571245528637</v>
       </c>
     </row>
     <row r="55">
@@ -1483,16 +1483,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>-0.050583382112964932</v>
+        <v>-0.051037037660406598</v>
       </c>
       <c r="C55">
-        <v>0.0097189999326566072</v>
+        <v>0.0097158463779240759</v>
       </c>
       <c r="D55">
-        <v>-0.069632424494905421</v>
+        <v>-0.070079905644939045</v>
       </c>
       <c r="E55">
-        <v>-0.031534339731024444</v>
+        <v>-0.031994169675874158</v>
       </c>
     </row>
     <row r="56">
@@ -1500,16 +1500,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>-0.17090609868618559</v>
+        <v>-0.17144930790708224</v>
       </c>
       <c r="C56">
-        <v>0.0037001168610596969</v>
+        <v>0.0038739281679304048</v>
       </c>
       <c r="D56">
-        <v>-0.17815820286158335</v>
+        <v>-0.17904207673267233</v>
       </c>
       <c r="E56">
-        <v>-0.16365399451078783</v>
+        <v>-0.16385653908149214</v>
       </c>
     </row>
     <row r="57">
@@ -1517,16 +1517,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>-0.016028626061704968</v>
+        <v>-0.015737008247020991</v>
       </c>
       <c r="C57">
-        <v>0.0071690196754307057</v>
+        <v>0.0085130994060001585</v>
       </c>
       <c r="D57">
-        <v>-0.030079662684048276</v>
+        <v>-0.032422396560134618</v>
       </c>
       <c r="E57">
-        <v>-0.00197758943936166</v>
+        <v>0.00094838006609263698</v>
       </c>
     </row>
     <row r="58">
@@ -1534,16 +1534,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>-0.046441167124778936</v>
+        <v>-0.046188137231600729</v>
       </c>
       <c r="C58">
-        <v>0.0048512632412930591</v>
+        <v>0.0056457324827623645</v>
       </c>
       <c r="D58">
-        <v>-0.055949479356317257</v>
+        <v>-0.057253582881213926</v>
       </c>
       <c r="E58">
-        <v>-0.036932854893240614</v>
+        <v>-0.035122691581987532</v>
       </c>
     </row>
     <row r="59">
@@ -1551,16 +1551,16 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>-0.072864874021992862</v>
+        <v>-0.072715277309320106</v>
       </c>
       <c r="C59">
-        <v>0.0027890271782769409</v>
+        <v>0.0027959752860964469</v>
       </c>
       <c r="D59">
-        <v>-0.078331273096040877</v>
+        <v>-0.078195294707612564</v>
       </c>
       <c r="E59">
-        <v>-0.067398474947944848</v>
+        <v>-0.067235259911027648</v>
       </c>
     </row>
     <row r="60">
@@ -1568,16 +1568,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>-0.062963825435666629</v>
+        <v>-0.062451558580310193</v>
       </c>
       <c r="C60">
-        <v>0.0073165483135899812</v>
+        <v>0.0069497810506852385</v>
       </c>
       <c r="D60">
-        <v>-0.077304013024424675</v>
+        <v>-0.076072895385919062</v>
       </c>
       <c r="E60">
-        <v>-0.048623637846908582</v>
+        <v>-0.048830221774701324</v>
       </c>
     </row>
     <row r="61">
@@ -1585,16 +1585,16 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>-0.070088971776455455</v>
+        <v>-0.070524948720959824</v>
       </c>
       <c r="C61">
-        <v>0.0045332364279093932</v>
+        <v>0.0041267250004946351</v>
       </c>
       <c r="D61">
-        <v>-0.078973962071628559</v>
+        <v>-0.078613190742673797</v>
       </c>
       <c r="E61">
-        <v>-0.061203981481282352</v>
+        <v>-0.06243670669924585</v>
       </c>
     </row>
     <row r="62">
@@ -1602,16 +1602,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>-0.18745343538691561</v>
+        <v>-0.18848955537043469</v>
       </c>
       <c r="C62">
-        <v>0.0042335225598879736</v>
+        <v>0.0047986840395332847</v>
       </c>
       <c r="D62">
-        <v>-0.19575099880757385</v>
+        <v>-0.19789481704683176</v>
       </c>
       <c r="E62">
-        <v>-0.17915587196625737</v>
+        <v>-0.17908429369403761</v>
       </c>
     </row>
     <row r="63">
@@ -1619,16 +1619,16 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>-0.031676969108568737</v>
+        <v>-0.03406779113727041</v>
       </c>
       <c r="C63">
-        <v>0.0080421036135629852</v>
+        <v>0.0077615652985257196</v>
       </c>
       <c r="D63">
-        <v>-0.047439224730234639</v>
+        <v>-0.049280201883566861</v>
       </c>
       <c r="E63">
-        <v>-0.015914713486902838</v>
+        <v>-0.01885538039097396</v>
       </c>
     </row>
     <row r="64">
@@ -1636,16 +1636,16 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>-0.032277904554026945</v>
+        <v>-0.031905699422267168</v>
       </c>
       <c r="C64">
-        <v>0.0057522289837011274</v>
+        <v>0.0061097490347398484</v>
       </c>
       <c r="D64">
-        <v>-0.043552082056856067</v>
+        <v>-0.043880605037105606</v>
       </c>
       <c r="E64">
-        <v>-0.02100372705119782</v>
+        <v>-0.01993079380742873</v>
       </c>
     </row>
     <row r="65">
@@ -1653,16 +1653,16 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>-0.095586051180981721</v>
+        <v>-0.095879266145450323</v>
       </c>
       <c r="C65">
-        <v>0.0031706245147574284</v>
+        <v>0.0033530772858844271</v>
       </c>
       <c r="D65">
-        <v>-0.10180036934722458</v>
+        <v>-0.10245118602571048</v>
       </c>
       <c r="E65">
-        <v>-0.089371733014738858</v>
+        <v>-0.089307346265190171</v>
       </c>
     </row>
     <row r="66">
@@ -1670,16 +1670,16 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>-0.067132165704782684</v>
+        <v>-0.06813287713407376</v>
       </c>
       <c r="C66">
-        <v>0.0074802091960400495</v>
+        <v>0.010053668452095835</v>
       </c>
       <c r="D66">
-        <v>-0.081793125928199428</v>
+        <v>-0.087837732685127776</v>
       </c>
       <c r="E66">
-        <v>-0.052471205481365947</v>
+        <v>-0.048428021583019745</v>
       </c>
     </row>
     <row r="67">
@@ -1687,16 +1687,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>-0.049052467251709329</v>
+        <v>-0.048943302561270045</v>
       </c>
       <c r="C67">
-        <v>0.004613208819104998</v>
+        <v>0.0041681730265395603</v>
       </c>
       <c r="D67">
-        <v>-0.058094202479517999</v>
+        <v>-0.057112782964479462</v>
       </c>
       <c r="E67">
-        <v>-0.040010732023900659</v>
+        <v>-0.040773822158060628</v>
       </c>
     </row>
     <row r="68">
@@ -1704,16 +1704,16 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>-0.13529941716211139</v>
+        <v>-0.13605383373896346</v>
       </c>
       <c r="C68">
-        <v>0.004706144437971794</v>
+        <v>0.0054461370151228433</v>
       </c>
       <c r="D68">
-        <v>-0.14452335127027313</v>
+        <v>-0.14672813857727882</v>
       </c>
       <c r="E68">
-        <v>-0.12607548305394964</v>
+        <v>-0.1253795289006481</v>
       </c>
     </row>
     <row r="69">
@@ -1721,16 +1721,16 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>-0.032284790343936956</v>
+        <v>-0.028636728849571125</v>
       </c>
       <c r="C69">
-        <v>0.015072976545456321</v>
+        <v>0.015156989110486447</v>
       </c>
       <c r="D69">
-        <v>-0.061827475295841074</v>
+        <v>-0.058344083208651525</v>
       </c>
       <c r="E69">
-        <v>-0.0027421053920328384</v>
+        <v>0.0010706255095092737</v>
       </c>
     </row>
     <row r="70">
@@ -1738,16 +1738,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>-0.027688696393671441</v>
+        <v>-0.027705096662575677</v>
       </c>
       <c r="C70">
-        <v>0.0087842270072979404</v>
+        <v>0.010484686296004591</v>
       </c>
       <c r="D70">
-        <v>-0.044905577892822887</v>
+        <v>-0.048254843638623091</v>
       </c>
       <c r="E70">
-        <v>-0.010471814894519996</v>
+        <v>-0.0071553496865282597</v>
       </c>
     </row>
     <row r="71">
@@ -1755,16 +1755,16 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>-0.048728794934438949</v>
+        <v>-0.048740900917380404</v>
       </c>
       <c r="C71">
-        <v>0.0052487731634228941</v>
+        <v>0.0054587678060659776</v>
       </c>
       <c r="D71">
-        <v>-0.059016283681843917</v>
+        <v>-0.059439978552584913</v>
       </c>
       <c r="E71">
-        <v>-0.03844130618703398</v>
+        <v>-0.038041823282175896</v>
       </c>
     </row>
     <row r="72">
@@ -1772,16 +1772,16 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>-0.037167619874071973</v>
+        <v>-0.03730727077361682</v>
       </c>
       <c r="C72">
-        <v>0.01898940935286355</v>
+        <v>0.019383329099734073</v>
       </c>
       <c r="D72">
-        <v>-0.074386476348725625</v>
+        <v>-0.075298214927043042</v>
       </c>
       <c r="E72">
-        <v>5.1236600581677783e-05</v>
+        <v>0.0006836733798094019</v>
       </c>
     </row>
     <row r="73">
@@ -1789,16 +1789,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>-0.019926549346050444</v>
+        <v>-0.019905694769312192</v>
       </c>
       <c r="C73">
-        <v>0.010012213003942564</v>
+        <v>0.008912672626692866</v>
       </c>
       <c r="D73">
-        <v>-0.039550283389742841</v>
+        <v>-0.037374357983780582</v>
       </c>
       <c r="E73">
-        <v>-0.00030281530235804974</v>
+        <v>-0.0024370315548438055</v>
       </c>
     </row>
     <row r="74">
@@ -1806,16 +1806,16 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>-0.16219774824889008</v>
+        <v>-0.1624344832649717</v>
       </c>
       <c r="C74">
-        <v>0.0035265420913925868</v>
+        <v>0.0035397020446388391</v>
       </c>
       <c r="D74">
-        <v>-0.16910965173357614</v>
+        <v>-0.16937218013785141</v>
       </c>
       <c r="E74">
-        <v>-0.15528584476420401</v>
+        <v>-0.155496786392092</v>
       </c>
     </row>
     <row r="75">
@@ -1823,16 +1823,16 @@
         <v>78</v>
       </c>
       <c r="B75">
-        <v>-0.014195553482730031</v>
+        <v>-0.011542933690666092</v>
       </c>
       <c r="C75">
-        <v>0.00828433273283531</v>
+        <v>0.0074366606297227734</v>
       </c>
       <c r="D75">
-        <v>-0.030432566057779629</v>
+        <v>-0.026118538231629476</v>
       </c>
       <c r="E75">
-        <v>0.0020414590923195693</v>
+        <v>0.0030326708502972921</v>
       </c>
     </row>
     <row r="76">
@@ -1840,16 +1840,16 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>-0.019864034707284851</v>
+        <v>-0.019803762997838252</v>
       </c>
       <c r="C76">
-        <v>0.0045546214110890378</v>
+        <v>0.0051612056787605481</v>
       </c>
       <c r="D76">
-        <v>-0.028790938962750735</v>
+        <v>-0.029919552419170582</v>
       </c>
       <c r="E76">
-        <v>-0.010937130451818966</v>
+        <v>-0.0096879735765059219</v>
       </c>
     </row>
     <row r="77">
@@ -1857,16 +1857,16 @@
         <v>80</v>
       </c>
       <c r="B77">
-        <v>-0.077170331265069766</v>
+        <v>-0.077207846274171266</v>
       </c>
       <c r="C77">
-        <v>0.0026569571678429975</v>
+        <v>0.0029001798261944628</v>
       </c>
       <c r="D77">
-        <v>-0.082377877579141584</v>
+        <v>-0.082892101061670206</v>
       </c>
       <c r="E77">
-        <v>-0.071962784950997949</v>
+        <v>-0.071523591486672325</v>
       </c>
     </row>
     <row r="78">
@@ -1874,16 +1874,16 @@
         <v>81</v>
       </c>
       <c r="B78">
-        <v>-0.072641814190882933</v>
+        <v>-0.072083475936214669</v>
       </c>
       <c r="C78">
-        <v>0.0063888164188598178</v>
+        <v>0.0079120562349799146</v>
       </c>
       <c r="D78">
-        <v>-0.08516367859877802</v>
+        <v>-0.087590839695674799</v>
       </c>
       <c r="E78">
-        <v>-0.060119949782987847</v>
+        <v>-0.056576112176754532</v>
       </c>
     </row>
     <row r="79">
@@ -1891,16 +1891,16 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>-0.05631821749182607</v>
+        <v>-0.056396522823466036</v>
       </c>
       <c r="C79">
-        <v>0.0037338256782667159</v>
+        <v>0.0039095820934436018</v>
       </c>
       <c r="D79">
-        <v>-0.063636389716645883</v>
+        <v>-0.064059172060267816</v>
       </c>
       <c r="E79">
-        <v>-0.049000045267006256</v>
+        <v>-0.048733873586664256</v>
       </c>
     </row>
     <row r="80">
@@ -1908,16 +1908,16 @@
         <v>83</v>
       </c>
       <c r="B80">
-        <v>-0.18642518927392587</v>
+        <v>-0.18660294874863606</v>
       </c>
       <c r="C80">
-        <v>0.0043983728177214888</v>
+        <v>0.0043361007160796425</v>
       </c>
       <c r="D80">
-        <v>-0.19504585371741689</v>
+        <v>-0.19510156244229951</v>
       </c>
       <c r="E80">
-        <v>-0.17780452483043485</v>
+        <v>-0.17810433505497261</v>
       </c>
     </row>
     <row r="81">
@@ -1925,16 +1925,16 @@
         <v>84</v>
       </c>
       <c r="B81">
-        <v>-0.0229729570982233</v>
+        <v>-0.024194431447557164</v>
       </c>
       <c r="C81">
-        <v>0.0088093724648378707</v>
+        <v>0.0085047571660458558</v>
       </c>
       <c r="D81">
-        <v>-0.040239034150881509</v>
+        <v>-0.040863473622847833</v>
       </c>
       <c r="E81">
-        <v>-0.0057068800455650909</v>
+        <v>-0.0075253892722664945</v>
       </c>
     </row>
     <row r="82">
@@ -1942,16 +1942,16 @@
         <v>85</v>
       </c>
       <c r="B82">
-        <v>-0.0090331675110519281</v>
+        <v>-0.0090544349058575696</v>
       </c>
       <c r="C82">
-        <v>0.0051514038919404648</v>
+        <v>0.0055124280534804872</v>
       </c>
       <c r="D82">
-        <v>-0.019129747816019699</v>
+        <v>-0.01985861119422571</v>
       </c>
       <c r="E82">
-        <v>0.0010634127939158442</v>
+        <v>0.0017497413825105727</v>
       </c>
     </row>
     <row r="83">
@@ -1959,16 +1959,16 @@
         <v>86</v>
       </c>
       <c r="B83">
-        <v>-0.1056454855571527</v>
+        <v>-0.1059623864036237</v>
       </c>
       <c r="C83">
-        <v>0.0036897760015928123</v>
+        <v>0.0034906405639863712</v>
       </c>
       <c r="D83">
-        <v>-0.11287732330058206</v>
+        <v>-0.1128039257304614</v>
       </c>
       <c r="E83">
-        <v>-0.098413647813723332</v>
+        <v>-0.099120847076785992</v>
       </c>
     </row>
     <row r="84">
@@ -1976,16 +1976,16 @@
         <v>87</v>
       </c>
       <c r="B84">
-        <v>-0.083307239596331378</v>
+        <v>-0.083831277632123641</v>
       </c>
       <c r="C84">
-        <v>0.0073214823145982318</v>
+        <v>0.0075415724947437875</v>
       </c>
       <c r="D84">
-        <v>-0.097657100432790134</v>
+        <v>-0.09861250871655923</v>
       </c>
       <c r="E84">
-        <v>-0.068957378759872623</v>
+        <v>-0.069050046547688052</v>
       </c>
     </row>
     <row r="85">
@@ -1993,16 +1993,16 @@
         <v>88</v>
       </c>
       <c r="B85">
-        <v>-0.038242629023473064</v>
+        <v>-0.038143550833410159</v>
       </c>
       <c r="C85">
-        <v>0.0045201256328233803</v>
+        <v>0.0045858760558330821</v>
       </c>
       <c r="D85">
-        <v>-0.047101924314673256</v>
+        <v>-0.047131715271674535</v>
       </c>
       <c r="E85">
-        <v>-0.029383333732272872</v>
+        <v>-0.029155386395145783</v>
       </c>
     </row>
     <row r="86">
@@ -2010,16 +2010,16 @@
         <v>89</v>
       </c>
       <c r="B86">
-        <v>-0.11911619303173704</v>
+        <v>-0.11926553768050896</v>
       </c>
       <c r="C86">
-        <v>0.0039577406532420156</v>
+        <v>0.0045246987951014792</v>
       </c>
       <c r="D86">
-        <v>-0.12687327305421725</v>
+        <v>-0.12813384453844467</v>
       </c>
       <c r="E86">
-        <v>-0.11135911300925683</v>
+        <v>-0.11039723082257326</v>
       </c>
     </row>
     <row r="87">
@@ -2027,16 +2027,16 @@
         <v>90</v>
       </c>
       <c r="B87">
-        <v>-0.039558460227922337</v>
+        <v>-0.042853997742438706</v>
       </c>
       <c r="C87">
-        <v>0.012256610032374745</v>
+        <v>0.013526658254311895</v>
       </c>
       <c r="D87">
-        <v>-0.063581132038815963</v>
+        <v>-0.069365940657077824</v>
       </c>
       <c r="E87">
-        <v>-0.015535788417028708</v>
+        <v>-0.016342054827799594</v>
       </c>
     </row>
     <row r="88">
@@ -2044,16 +2044,16 @@
         <v>91</v>
       </c>
       <c r="B88">
-        <v>-0.01259052575459811</v>
+        <v>-0.012258053450968439</v>
       </c>
       <c r="C88">
-        <v>0.007562783422633685</v>
+        <v>0.0070129005935404875</v>
       </c>
       <c r="D88">
-        <v>-0.027413406115391913</v>
+        <v>-0.026003179313279376</v>
       </c>
       <c r="E88">
-        <v>0.0022323546061956915</v>
+        <v>0.001487072411342499</v>
       </c>
     </row>
     <row r="89">
@@ -2061,16 +2061,16 @@
         <v>92</v>
       </c>
       <c r="B89">
-        <v>-0.051253953251608281</v>
+        <v>-0.050869441297018515</v>
       </c>
       <c r="C89">
-        <v>0.0050540400484021721</v>
+        <v>0.0048548053378738576</v>
       </c>
       <c r="D89">
-        <v>-0.061159769050469145</v>
+        <v>-0.060384764362417617</v>
       </c>
       <c r="E89">
-        <v>-0.041348137452747416</v>
+        <v>-0.041354118231619413</v>
       </c>
     </row>
     <row r="90">
@@ -2078,16 +2078,16 @@
         <v>93</v>
       </c>
       <c r="B90">
-        <v>-0.07114735465277236</v>
+        <v>-0.071853694117320677</v>
       </c>
       <c r="C90">
-        <v>0.017033356253932305</v>
+        <v>0.016256202261049648</v>
       </c>
       <c r="D90">
-        <v>-0.10453238679971225</v>
+        <v>-0.10371553111490904</v>
       </c>
       <c r="E90">
-        <v>-0.037762322505832467</v>
+        <v>-0.039991857119732313</v>
       </c>
     </row>
     <row r="91">
@@ -2095,16 +2095,16 @@
         <v>94</v>
       </c>
       <c r="B91">
-        <v>0.0071171857779218873</v>
+        <v>0.007142810012217669</v>
       </c>
       <c r="C91">
-        <v>0.0094081711797711371</v>
+        <v>0.010284359587270919</v>
       </c>
       <c r="D91">
-        <v>-0.011322638564275019</v>
+        <v>-0.013014332691360703</v>
       </c>
       <c r="E91">
-        <v>0.025557010120118795</v>
+        <v>0.027299952715796043</v>
       </c>
     </row>
     <row r="92">
@@ -2112,16 +2112,16 @@
         <v>95</v>
       </c>
       <c r="B92">
-        <v>-0.15382355388367205</v>
+        <v>-0.15359411826640459</v>
       </c>
       <c r="C92">
-        <v>0.0035882474733497085</v>
+        <v>0.0030447165458126115</v>
       </c>
       <c r="D92">
-        <v>-0.16085639783454858</v>
+        <v>-0.15956166022115251</v>
       </c>
       <c r="E92">
-        <v>-0.14679070993279553</v>
+        <v>-0.14762657631165668</v>
       </c>
     </row>
     <row r="93">
@@ -2129,16 +2129,16 @@
         <v>96</v>
       </c>
       <c r="B93">
-        <v>-0.0030759845120480142</v>
+        <v>-0.0051561944649184269</v>
       </c>
       <c r="C93">
-        <v>0.0074203226849343601</v>
+        <v>0.007205797160212417</v>
       </c>
       <c r="D93">
-        <v>-0.017619566551994575</v>
+        <v>-0.019279314375739001</v>
       </c>
       <c r="E93">
-        <v>0.011467597527898546</v>
+        <v>0.0089669254459021457</v>
       </c>
     </row>
     <row r="94">
@@ -2146,16 +2146,16 @@
         <v>97</v>
       </c>
       <c r="B94">
-        <v>0.0051011908721357267</v>
+        <v>0.0050401794508542659</v>
       </c>
       <c r="C94">
-        <v>0.0043403407982462016</v>
+        <v>0.0044046645829852946</v>
       </c>
       <c r="D94">
-        <v>-0.0034057306137429116</v>
+        <v>-0.0035928148854187276</v>
       </c>
       <c r="E94">
-        <v>0.013608112358014365</v>
+        <v>0.013673173787127259</v>
       </c>
     </row>
     <row r="95">
@@ -2163,16 +2163,16 @@
         <v>98</v>
       </c>
       <c r="B95">
-        <v>-0.078756351762687804</v>
+        <v>-0.07887355483997488</v>
       </c>
       <c r="C95">
-        <v>0.0029232584449172629</v>
+        <v>0.0025339711344798243</v>
       </c>
       <c r="D95">
-        <v>-0.08448583958588321</v>
+        <v>-0.083840052924837177</v>
       </c>
       <c r="E95">
-        <v>-0.073026863939492398</v>
+        <v>-0.073907056755112582</v>
       </c>
     </row>
     <row r="96">
@@ -2180,16 +2180,16 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>-0.068137712191966959</v>
+        <v>-0.068227267816337506</v>
       </c>
       <c r="C96">
-        <v>0.0075409455656702184</v>
+        <v>0.0073248104547497094</v>
       </c>
       <c r="D96">
-        <v>-0.082917710816108367</v>
+        <v>-0.082583649623725996</v>
       </c>
       <c r="E96">
-        <v>-0.053357713567825552</v>
+        <v>-0.053870886008949008</v>
       </c>
     </row>
     <row r="97">
@@ -2197,16 +2197,16 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>-0.037599674274464916</v>
+        <v>-0.037557579073190253</v>
       </c>
       <c r="C97">
-        <v>0.0039118457314735343</v>
+        <v>0.0037103151489467495</v>
       </c>
       <c r="D97">
-        <v>-0.045266759791199269</v>
+        <v>-0.044829671809661915</v>
       </c>
       <c r="E97">
-        <v>-0.029932588757730562</v>
+        <v>-0.030285486336718591</v>
       </c>
     </row>
     <row r="98">
@@ -2214,16 +2214,16 @@
         <v>101</v>
       </c>
       <c r="B98">
-        <v>-0.18181319995626377</v>
+        <v>-0.18144145461410588</v>
       </c>
       <c r="C98">
-        <v>0.0042001489642820916</v>
+        <v>0.0046103064380590766</v>
       </c>
       <c r="D98">
-        <v>-0.19004535223945956</v>
+        <v>-0.19047750243494574</v>
       </c>
       <c r="E98">
-        <v>-0.17358104767306798</v>
+        <v>-0.17240540679326602</v>
       </c>
     </row>
     <row r="99">
@@ -2231,16 +2231,16 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>-0.0034166226936080124</v>
+        <v>-0.0038256090242376212</v>
       </c>
       <c r="C99">
-        <v>0.0093265028718005055</v>
+        <v>0.0090897827272033351</v>
       </c>
       <c r="D99">
-        <v>-0.021696258145406253</v>
+        <v>-0.021641281910101659</v>
       </c>
       <c r="E99">
-        <v>0.014863012758190228</v>
+        <v>0.013990063861626415</v>
       </c>
     </row>
     <row r="100">
@@ -2248,16 +2248,16 @@
         <v>103</v>
       </c>
       <c r="B100">
-        <v>0.01943247576105293</v>
+        <v>0.019610057085003324</v>
       </c>
       <c r="C100">
-        <v>0.0049829600106568814</v>
+        <v>0.0056642757540632188</v>
       </c>
       <c r="D100">
-        <v>0.009666039861364847</v>
+        <v>0.0085082643361276689</v>
       </c>
       <c r="E100">
-        <v>0.029198911660741012</v>
+        <v>0.030711849833878979</v>
       </c>
     </row>
     <row r="101">
@@ -2265,16 +2265,16 @@
         <v>104</v>
       </c>
       <c r="B101">
-        <v>-0.10991140068411474</v>
+        <v>-0.11008008286954568</v>
       </c>
       <c r="C101">
-        <v>0.0032553250457699064</v>
+        <v>0.003875250170748802</v>
       </c>
       <c r="D101">
-        <v>-0.1162917290625765</v>
+        <v>-0.11767544422472186</v>
       </c>
       <c r="E101">
-        <v>-0.10353107230565299</v>
+        <v>-0.10248472151436951</v>
       </c>
     </row>
     <row r="102">
@@ -2282,16 +2282,16 @@
         <v>105</v>
       </c>
       <c r="B102">
-        <v>-0.069282565869227639</v>
+        <v>-0.06932299432085931</v>
       </c>
       <c r="C102">
-        <v>0.0073516554257444279</v>
+        <v>0.0080093651361275546</v>
       </c>
       <c r="D102">
-        <v>-0.08369156499590498</v>
+        <v>-0.085021083412920126</v>
       </c>
       <c r="E102">
-        <v>-0.054873566742550298</v>
+        <v>-0.053624905228798495</v>
       </c>
     </row>
     <row r="103">
@@ -2299,16 +2299,16 @@
         <v>106</v>
       </c>
       <c r="B103">
-        <v>-0.024857887229033274</v>
+        <v>-0.024776551409079032</v>
       </c>
       <c r="C103">
-        <v>0.0041623609234634693</v>
+        <v>0.0046043241870081762</v>
       </c>
       <c r="D103">
-        <v>-0.033015975637403952</v>
+        <v>-0.033800873570439628</v>
       </c>
       <c r="E103">
-        <v>-0.016699798820662595</v>
+        <v>-0.015752229247718436</v>
       </c>
     </row>
     <row r="104">
@@ -2316,16 +2316,16 @@
         <v>107</v>
       </c>
       <c r="B104">
-        <v>-0.10999072782150629</v>
+        <v>-0.10986104106516713</v>
       </c>
       <c r="C104">
-        <v>0.004393184115271306</v>
+        <v>0.0038497913548884541</v>
       </c>
       <c r="D104">
-        <v>-0.11860126694506734</v>
+        <v>-0.11740654467109569</v>
       </c>
       <c r="E104">
-        <v>-0.10138018869794524</v>
+        <v>-0.10231553745923856</v>
       </c>
     </row>
     <row r="105">
@@ -2333,16 +2333,16 @@
         <v>108</v>
       </c>
       <c r="B105">
-        <v>-0.056965513535319263</v>
+        <v>-0.058448558341902428</v>
       </c>
       <c r="C105">
-        <v>0.012142764290975895</v>
+        <v>0.01112844829457907</v>
       </c>
       <c r="D105">
-        <v>-0.080765050329640736</v>
+        <v>-0.080260064211827423</v>
       </c>
       <c r="E105">
-        <v>-0.033165976740997791</v>
+        <v>-0.036637052471977433</v>
       </c>
     </row>
     <row r="106">
@@ -2350,16 +2350,16 @@
         <v>109</v>
       </c>
       <c r="B106">
-        <v>0.0066547266346321911</v>
+        <v>0.0071395342878408539</v>
       </c>
       <c r="C106">
-        <v>0.0073193382110774861</v>
+        <v>0.0064120654216631963</v>
       </c>
       <c r="D106">
-        <v>-0.007691006749493458</v>
+        <v>-0.0054279682858178165</v>
       </c>
       <c r="E106">
-        <v>0.021000460018757841</v>
+        <v>0.019707036861499525</v>
       </c>
     </row>
     <row r="107">
@@ -2367,16 +2367,16 @@
         <v>110</v>
       </c>
       <c r="B107">
-        <v>-0.058407681973055389</v>
+        <v>-0.05822893798416922</v>
       </c>
       <c r="C107">
-        <v>0.0054062717117544304</v>
+        <v>0.0053440597599996708</v>
       </c>
       <c r="D107">
-        <v>-0.069003864674884688</v>
+        <v>-0.068703190103094711</v>
       </c>
       <c r="E107">
-        <v>-0.047811499271226091</v>
+        <v>-0.047754685865243729</v>
       </c>
     </row>
     <row r="108">
@@ -2384,16 +2384,16 @@
         <v>111</v>
       </c>
       <c r="B108">
-        <v>-0.077941056354496469</v>
+        <v>-0.078865046983383216</v>
       </c>
       <c r="C108">
-        <v>0.016764172434884195</v>
+        <v>0.015939042022954684</v>
       </c>
       <c r="D108">
-        <v>-0.11079849368580615</v>
+        <v>-0.11010525614649817</v>
       </c>
       <c r="E108">
-        <v>-0.045083619023186791</v>
+        <v>-0.047624837820268259</v>
       </c>
     </row>
     <row r="109">
@@ -2401,16 +2401,16 @@
         <v>112</v>
       </c>
       <c r="B109">
-        <v>0.032511706725408866</v>
+        <v>0.032250219225038457</v>
       </c>
       <c r="C109">
-        <v>0.0096314444946049051</v>
+        <v>0.0095000549553185681</v>
       </c>
       <c r="D109">
-        <v>0.013634271222959363</v>
+        <v>0.013630298188515411</v>
       </c>
       <c r="E109">
-        <v>0.05138914222785837</v>
+        <v>0.050870140261561503</v>
       </c>
     </row>
     <row r="110">
@@ -2418,16 +2418,16 @@
         <v>113</v>
       </c>
       <c r="B110">
-        <v>-0.15127679311551917</v>
+        <v>-0.1508544738641007</v>
       </c>
       <c r="C110">
-        <v>0.0032963572056500688</v>
+        <v>0.0035891242579184301</v>
       </c>
       <c r="D110">
-        <v>-0.15773754199247517</v>
+        <v>-0.15788903661162088</v>
       </c>
       <c r="E110">
-        <v>-0.14481604423856317</v>
+        <v>-0.14381991111658052</v>
       </c>
     </row>
     <row r="111">
@@ -2435,16 +2435,16 @@
         <v>114</v>
       </c>
       <c r="B111">
-        <v>-0.019707089056676053</v>
+        <v>-0.017505115853076667</v>
       </c>
       <c r="C111">
-        <v>0.0070101136251367741</v>
+        <v>0.0078373515095326307</v>
       </c>
       <c r="D111">
-        <v>-0.033446675183236227</v>
+        <v>-0.032866061032543394</v>
       </c>
       <c r="E111">
-        <v>-0.0059675029301158831</v>
+        <v>-0.0021441706736099377</v>
       </c>
     </row>
     <row r="112">
@@ -2452,16 +2452,16 @@
         <v>115</v>
       </c>
       <c r="B112">
-        <v>0.029983112855325355</v>
+        <v>0.030536759022870948</v>
       </c>
       <c r="C112">
-        <v>0.0039386368565210751</v>
+        <v>0.0047838850004588663</v>
       </c>
       <c r="D112">
-        <v>0.022263517538443502</v>
+        <v>0.021160505431649289</v>
       </c>
       <c r="E112">
-        <v>0.037702708172207208</v>
+        <v>0.039913012614092608</v>
       </c>
     </row>
     <row r="113">
@@ -2469,16 +2469,16 @@
         <v>116</v>
       </c>
       <c r="B113">
-        <v>-0.085809422285161169</v>
+        <v>-0.085730502480827073</v>
       </c>
       <c r="C113">
-        <v>0.0030580226128252503</v>
+        <v>0.0035377491434974112</v>
       </c>
       <c r="D113">
-        <v>-0.09180304332599061</v>
+        <v>-0.092664371658271336</v>
       </c>
       <c r="E113">
-        <v>-0.079815801244331727</v>
+        <v>-0.07879663330338281</v>
       </c>
     </row>
     <row r="114">
@@ -2486,16 +2486,16 @@
         <v>117</v>
       </c>
       <c r="B114">
-        <v>-0.055841271150374808</v>
+        <v>-0.054939497133350217</v>
       </c>
       <c r="C114">
-        <v>0.0082102874835953236</v>
+        <v>0.0077526115876319227</v>
       </c>
       <c r="D114">
-        <v>-0.071933157327590466</v>
+        <v>-0.070134354753762368</v>
       </c>
       <c r="E114">
-        <v>-0.039749384973159149</v>
+        <v>-0.039744639512938072</v>
       </c>
     </row>
     <row r="115">
@@ -2503,16 +2503,16 @@
         <v>118</v>
       </c>
       <c r="B115">
-        <v>-0.014296175935988545</v>
+        <v>-0.013803169841201177</v>
       </c>
       <c r="C115">
-        <v>0.0044130050190720593</v>
+        <v>0.0041087009324844975</v>
       </c>
       <c r="D115">
-        <v>-0.02294551673048309</v>
+        <v>-0.021856085296627276</v>
       </c>
       <c r="E115">
-        <v>-0.0056468351414939982</v>
+        <v>-0.0057502543857750801</v>
       </c>
     </row>
     <row r="116">
@@ -2520,16 +2520,16 @@
         <v>119</v>
       </c>
       <c r="B116">
-        <v>-0.17428207879786398</v>
+        <v>-0.17452127890727442</v>
       </c>
       <c r="C116">
-        <v>0.0046293748451450394</v>
+        <v>0.0042401726443421928</v>
       </c>
       <c r="D116">
-        <v>-0.18335549953253635</v>
+        <v>-0.18283187675964263</v>
       </c>
       <c r="E116">
-        <v>-0.1652086580631916</v>
+        <v>-0.16621068105490622</v>
       </c>
     </row>
     <row r="117">
@@ -2537,16 +2537,16 @@
         <v>120</v>
       </c>
       <c r="B117">
-        <v>-8.8381508670713088e-05</v>
+        <v>-0.0014914052304718479</v>
       </c>
       <c r="C117">
-        <v>0.0093567183187093558</v>
+        <v>0.0094310393683456877</v>
       </c>
       <c r="D117">
-        <v>-0.018427238231517606</v>
+        <v>-0.019975929822826716</v>
       </c>
       <c r="E117">
-        <v>0.018250475214176182</v>
+        <v>0.016993119361883021</v>
       </c>
     </row>
     <row r="118">
@@ -2554,16 +2554,16 @@
         <v>121</v>
       </c>
       <c r="B118">
-        <v>0.039156569447885557</v>
+        <v>0.04020375571442257</v>
       </c>
       <c r="C118">
-        <v>0.0056399618309522538</v>
+        <v>0.0055267080469438351</v>
       </c>
       <c r="D118">
-        <v>0.028102431830710227</v>
+        <v>0.02937159111214304</v>
       </c>
       <c r="E118">
-        <v>0.050210707065060887</v>
+        <v>0.051035920316702101</v>
       </c>
     </row>
     <row r="119">
@@ -2571,16 +2571,16 @@
         <v>122</v>
       </c>
       <c r="B119">
-        <v>-0.10894087081167317</v>
+        <v>-0.10898057283034132</v>
       </c>
       <c r="C119">
-        <v>0.0040893521985196956</v>
+        <v>0.0037203006075792349</v>
       </c>
       <c r="D119">
-        <v>-0.11695586455727296</v>
+        <v>-0.11627223819887306</v>
       </c>
       <c r="E119">
-        <v>-0.10092587706607338</v>
+        <v>-0.10168890746180959</v>
       </c>
     </row>
     <row r="120">
@@ -2588,16 +2588,16 @@
         <v>123</v>
       </c>
       <c r="B120">
-        <v>-0.055071721230367951</v>
+        <v>-0.053323570133972223</v>
       </c>
       <c r="C120">
-        <v>0.0077625092960273484</v>
+        <v>0.0081374573755566195</v>
       </c>
       <c r="D120">
-        <v>-0.070285980222376795</v>
+        <v>-0.06927271575203521</v>
       </c>
       <c r="E120">
-        <v>-0.0398574622383591</v>
+        <v>-0.037374424515909235</v>
       </c>
     </row>
     <row r="121">
@@ -2605,16 +2605,16 @@
         <v>124</v>
       </c>
       <c r="B121">
-        <v>-0.0087055048250453976</v>
+        <v>-0.0084886142435760988</v>
       </c>
       <c r="C121">
-        <v>0.0050282490482468417</v>
+        <v>0.0049322963962911198</v>
       </c>
       <c r="D121">
-        <v>-0.018560705041746037</v>
+        <v>-0.018155751019271152</v>
       </c>
       <c r="E121">
-        <v>0.0011496953916552421</v>
+        <v>0.0011785225321189544</v>
       </c>
     </row>
     <row r="122">
@@ -2622,16 +2622,16 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>-0.11491139530909911</v>
+        <v>-0.11419855844945782</v>
       </c>
       <c r="C122">
-        <v>0.0044031776263993754</v>
+        <v>0.0046195509610391129</v>
       </c>
       <c r="D122">
-        <v>-0.12354152148303005</v>
+        <v>-0.12325277339802387</v>
       </c>
       <c r="E122">
-        <v>-0.10628126913516817</v>
+        <v>-0.10514434350089177</v>
       </c>
     </row>
     <row r="123">
@@ -2639,16 +2639,16 @@
         <v>126</v>
       </c>
       <c r="B123">
-        <v>-0.080883521757762644</v>
+        <v>-0.078963863555763458</v>
       </c>
       <c r="C123">
-        <v>0.013320323233659333</v>
+        <v>0.013641201374092003</v>
       </c>
       <c r="D123">
-        <v>-0.10699104680848998</v>
+        <v>-0.10570030838327575</v>
       </c>
       <c r="E123">
-        <v>-0.054775996707035313</v>
+        <v>-0.052227418728251165</v>
       </c>
     </row>
     <row r="124">
@@ -2656,16 +2656,16 @@
         <v>127</v>
       </c>
       <c r="B124">
-        <v>0.028463289958035088</v>
+        <v>0.027264102762036006</v>
       </c>
       <c r="C124">
-        <v>0.0066284059351501218</v>
+        <v>0.008734518213695544</v>
       </c>
       <c r="D124">
-        <v>0.015471767833329019</v>
+        <v>0.010144645471499774</v>
       </c>
       <c r="E124">
-        <v>0.041454812082741155</v>
+        <v>0.044383560052572241</v>
       </c>
     </row>
     <row r="125">
@@ -2673,16 +2673,16 @@
         <v>128</v>
       </c>
       <c r="B125">
-        <v>-0.061806770252188462</v>
+        <v>-0.061452015761060907</v>
       </c>
       <c r="C125">
-        <v>0.0046738560447442557</v>
+        <v>0.0047305522680712196</v>
       </c>
       <c r="D125">
-        <v>-0.070967433129061813</v>
+        <v>-0.070723805251217325</v>
       </c>
       <c r="E125">
-        <v>-0.052646107375315103</v>
+        <v>-0.05218022627090449</v>
       </c>
     </row>
     <row r="126">
@@ -2690,16 +2690,16 @@
         <v>129</v>
       </c>
       <c r="B126">
-        <v>-0.094969097147558953</v>
+        <v>-0.090553392455784296</v>
       </c>
       <c r="C126">
-        <v>0.016449915997848775</v>
+        <v>0.018153253655766307</v>
       </c>
       <c r="D126">
-        <v>-0.12721059824784028</v>
+        <v>-0.12613341290999305</v>
       </c>
       <c r="E126">
-        <v>-0.062727596047277623</v>
+        <v>-0.054973372001575538</v>
       </c>
     </row>
     <row r="127">
@@ -2707,16 +2707,16 @@
         <v>130</v>
       </c>
       <c r="B127">
-        <v>0.063259206969419599</v>
+        <v>0.063627324821543069</v>
       </c>
       <c r="C127">
-        <v>0.0086628998951266585</v>
+        <v>0.0091036543810173159</v>
       </c>
       <c r="D127">
-        <v>0.046280099201521027</v>
+        <v>0.045784341121386643</v>
       </c>
       <c r="E127">
-        <v>0.08023831473731817</v>
+        <v>0.081470308521699494</v>
       </c>
     </row>
     <row r="128">
@@ -2724,16 +2724,16 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>-0.15025526547360829</v>
+        <v>-0.14878708002839006</v>
       </c>
       <c r="C128">
-        <v>0.0038795021884292496</v>
+        <v>0.0035238112046085813</v>
       </c>
       <c r="D128">
-        <v>-0.15785895883671869</v>
+        <v>-0.15569363138964334</v>
       </c>
       <c r="E128">
-        <v>-0.14265157211049789</v>
+        <v>-0.14188052866713677</v>
       </c>
     </row>
     <row r="129">
@@ -2741,16 +2741,16 @@
         <v>132</v>
       </c>
       <c r="B129">
-        <v>-0.010105223525071556</v>
+        <v>-0.0095749239663312294</v>
       </c>
       <c r="C129">
-        <v>0.0084990781394585786</v>
+        <v>0.0082974132615882563</v>
       </c>
       <c r="D129">
-        <v>-0.026763129849832097</v>
+        <v>-0.025837574695676671</v>
       </c>
       <c r="E129">
-        <v>0.0065526827996889858</v>
+        <v>0.0066877267630142123</v>
       </c>
     </row>
     <row r="130">
@@ -2758,16 +2758,16 @@
         <v>133</v>
       </c>
       <c r="B130">
-        <v>0.053548162414563553</v>
+        <v>0.053411118145023757</v>
       </c>
       <c r="C130">
-        <v>0.0047252610015633967</v>
+        <v>0.0040870959899471032</v>
       </c>
       <c r="D130">
-        <v>0.044286810320546738</v>
+        <v>0.045400547562801694</v>
       </c>
       <c r="E130">
-        <v>0.062809514508580369</v>
+        <v>0.061421688727245821</v>
       </c>
     </row>
     <row r="131">
@@ -2775,16 +2775,16 @@
         <v>134</v>
       </c>
       <c r="B131">
-        <v>-0.08549135257362063</v>
+        <v>-0.085461740411918313</v>
       </c>
       <c r="C131">
-        <v>0.0035025435278000904</v>
+        <v>0.0035561605225974098</v>
       </c>
       <c r="D131">
-        <v>-0.092356219594747282</v>
+        <v>-0.092431695272342768</v>
       </c>
       <c r="E131">
-        <v>-0.078626485552493977</v>
+        <v>-0.078491785551493859</v>
       </c>
     </row>
     <row r="132">
@@ -2792,16 +2792,16 @@
         <v>135</v>
       </c>
       <c r="B132">
-        <v>-0.058229813226220742</v>
+        <v>-0.058306484410707758</v>
       </c>
       <c r="C132">
-        <v>0.0074228990406370902</v>
+        <v>0.0083571647623407741</v>
       </c>
       <c r="D132">
-        <v>-0.072778444648148533</v>
+        <v>-0.074686245893493736</v>
       </c>
       <c r="E132">
-        <v>-0.043681181804292951</v>
+        <v>-0.041926722927921781</v>
       </c>
     </row>
     <row r="133">
@@ -2809,16 +2809,16 @@
         <v>136</v>
       </c>
       <c r="B133">
-        <v>0.011321490198088414</v>
+        <v>0.011789298860186984</v>
       </c>
       <c r="C133">
-        <v>0.0044081171888352682</v>
+        <v>0.0044476995472949891</v>
       </c>
       <c r="D133">
-        <v>0.002681729385778554</v>
+        <v>0.0030719575364792848</v>
       </c>
       <c r="E133">
-        <v>0.019961251010398272</v>
+        <v>0.020506640183894684</v>
       </c>
     </row>
     <row r="134">
@@ -2826,16 +2826,16 @@
         <v>137</v>
       </c>
       <c r="B134">
-        <v>-0.16269505558256042</v>
+        <v>-0.16212717337230881</v>
       </c>
       <c r="C134">
-        <v>0.0047523185765299368</v>
+        <v>0.0042990621547536233</v>
       </c>
       <c r="D134">
-        <v>-0.17200944194193601</v>
+        <v>-0.17055319271332919</v>
       </c>
       <c r="E134">
-        <v>-0.15338066922318483</v>
+        <v>-0.15370115403128842</v>
       </c>
     </row>
     <row r="135">
@@ -2843,16 +2843,16 @@
         <v>138</v>
       </c>
       <c r="B135">
-        <v>0.014050269395184082</v>
+        <v>0.013252183905347915</v>
       </c>
       <c r="C135">
-        <v>0.0091636874136343336</v>
+        <v>0.0085046811866671436</v>
       </c>
       <c r="D135">
-        <v>-0.0039102531734568537</v>
+        <v>-0.003416709352878633</v>
       </c>
       <c r="E135">
-        <v>0.032010791963825017</v>
+        <v>0.029921077163574464</v>
       </c>
     </row>
     <row r="136">
@@ -2860,16 +2860,16 @@
         <v>139</v>
       </c>
       <c r="B136">
-        <v>0.061787866332550373</v>
+        <v>0.061968224947103905</v>
       </c>
       <c r="C136">
-        <v>0.0055812586976380354</v>
+        <v>0.005385624481502543</v>
       </c>
       <c r="D136">
-        <v>0.050848784904346661</v>
+        <v>0.051412579457206592</v>
       </c>
       <c r="E136">
-        <v>0.072726947760754085</v>
+        <v>0.072523870437001217</v>
       </c>
     </row>
     <row r="137">
@@ -2877,16 +2877,16 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>-0.10435812858343708</v>
+        <v>-0.10344401413165762</v>
       </c>
       <c r="C137">
-        <v>0.0041547949579460453</v>
+        <v>0.004277916828969751</v>
       </c>
       <c r="D137">
-        <v>-0.11250138795205826</v>
+        <v>-0.11182858873504026</v>
       </c>
       <c r="E137">
-        <v>-0.09621486921481591</v>
+        <v>-0.095059439528274975</v>
       </c>
     </row>
     <row r="138">
@@ -2894,16 +2894,16 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>-0.050346591087030303</v>
+        <v>-0.051252233355707784</v>
       </c>
       <c r="C138">
-        <v>0.0097692660630309281</v>
+        <v>0.0090182846123186729</v>
       </c>
       <c r="D138">
-        <v>-0.069494026326928984</v>
+        <v>-0.068927771041356015</v>
       </c>
       <c r="E138">
-        <v>-0.031199155847131618</v>
+        <v>-0.033576695670059553</v>
       </c>
     </row>
     <row r="139">
@@ -2911,16 +2911,16 @@
         <v>142</v>
       </c>
       <c r="B139">
-        <v>0.00872168712547031</v>
+        <v>0.0079504258811163419</v>
       </c>
       <c r="C139">
-        <v>0.0053257665765504099</v>
+        <v>0.0055092764143110312</v>
       </c>
       <c r="D139">
-        <v>-0.0017166375111378664</v>
+        <v>-0.00284757252634028</v>
       </c>
       <c r="E139">
-        <v>0.019160011762078488</v>
+        <v>0.018748424288572964</v>
       </c>
     </row>
     <row r="140">
@@ -2928,16 +2928,16 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>-0.11181900843582392</v>
+        <v>-0.11104930437534498</v>
       </c>
       <c r="C140">
-        <v>0.0053078751613163345</v>
+        <v>0.0046271369425741372</v>
       </c>
       <c r="D140">
-        <v>-0.12222232082617425</v>
+        <v>-0.12011838767540088</v>
       </c>
       <c r="E140">
-        <v>-0.10141569604547358</v>
+        <v>-0.10198022107528908</v>
       </c>
     </row>
     <row r="141">
@@ -2945,16 +2945,16 @@
         <v>144</v>
       </c>
       <c r="B141">
-        <v>-0.071195730652949082</v>
+        <v>-0.071492286675496147</v>
       </c>
       <c r="C141">
-        <v>0.014702033096361566</v>
+        <v>0.016104929991012137</v>
       </c>
       <c r="D141">
-        <v>-0.10001137503535915</v>
+        <v>-0.10305758362752544</v>
       </c>
       <c r="E141">
-        <v>-0.042380086270539019</v>
+        <v>-0.039926989723466852</v>
       </c>
     </row>
     <row r="142">
@@ -2962,16 +2962,16 @@
         <v>145</v>
       </c>
       <c r="B142">
-        <v>0.038456720970424088</v>
+        <v>0.038655720455015044</v>
       </c>
       <c r="C142">
-        <v>0.0086071642549709285</v>
+        <v>0.0073937845983406631</v>
       </c>
       <c r="D142">
-        <v>0.021586878365212326</v>
+        <v>0.024164070595238403</v>
       </c>
       <c r="E142">
-        <v>0.055326563575635854</v>
+        <v>0.053147370314791685</v>
       </c>
     </row>
     <row r="143">
@@ -2979,16 +2979,16 @@
         <v>146</v>
       </c>
       <c r="B143">
-        <v>-0.066004740694341466</v>
+        <v>-0.065489781760245544</v>
       </c>
       <c r="C143">
-        <v>0.0059973388039176925</v>
+        <v>0.0064860069040179463</v>
       </c>
       <c r="D143">
-        <v>-0.077759402886571447</v>
+        <v>-0.078202227842206942</v>
       </c>
       <c r="E143">
-        <v>-0.054250078502111485</v>
+        <v>-0.052777335678284146</v>
       </c>
     </row>
     <row r="144">
@@ -2996,16 +2996,16 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>-0.13004351853451074</v>
+        <v>-0.12725315740913867</v>
       </c>
       <c r="C144">
-        <v>0.018636502938370932</v>
+        <v>0.018403647742613286</v>
       </c>
       <c r="D144">
-        <v>-0.16657068560767152</v>
+        <v>-0.16332394535332839</v>
       </c>
       <c r="E144">
-        <v>-0.093516351461349956</v>
+        <v>-0.09118236946494894</v>
       </c>
     </row>
     <row r="145">
@@ -3013,16 +3013,16 @@
         <v>148</v>
       </c>
       <c r="B145">
-        <v>0.068842339071144676</v>
+        <v>0.069203662115669085</v>
       </c>
       <c r="C145">
-        <v>0.0098116105224643167</v>
+        <v>0.0097908075251625596</v>
       </c>
       <c r="D145">
-        <v>0.049611781814990034</v>
+        <v>0.050013871755534352</v>
       </c>
       <c r="E145">
-        <v>0.08807289632729931</v>
+        <v>0.088393452475803824</v>
       </c>
     </row>
     <row r="146">
@@ -3030,16 +3030,16 @@
         <v>149</v>
       </c>
       <c r="B146">
-        <v>-0.13890103976959611</v>
+        <v>-0.13797266331141456</v>
       </c>
       <c r="C146">
-        <v>0.0035427636873311256</v>
+        <v>0.003789313962330195</v>
       </c>
       <c r="D146">
-        <v>-0.14584473703487205</v>
+        <v>-0.14539959114186135</v>
       </c>
       <c r="E146">
-        <v>-0.13195734250432017</v>
+        <v>-0.13054573548096776</v>
       </c>
     </row>
     <row r="147">
@@ -3047,16 +3047,16 @@
         <v>150</v>
       </c>
       <c r="B147">
-        <v>-0.0015533136095602243</v>
+        <v>-0.0041056968364420257</v>
       </c>
       <c r="C147">
-        <v>0.010596017955337661</v>
+        <v>0.010134118353898668</v>
       </c>
       <c r="D147">
-        <v>-0.022321151205502088</v>
+        <v>-0.023968227729323745</v>
       </c>
       <c r="E147">
-        <v>0.019214523986381637</v>
+        <v>0.015756834056439694</v>
       </c>
     </row>
     <row r="148">
@@ -3064,16 +3064,16 @@
         <v>151</v>
       </c>
       <c r="B148">
-        <v>0.069244725625008954</v>
+        <v>0.069168830036793971</v>
       </c>
       <c r="C148">
-        <v>0.004746342751216783</v>
+        <v>0.0050721618708152207</v>
       </c>
       <c r="D148">
-        <v>0.059942054013142579</v>
+        <v>0.059227563482115698</v>
       </c>
       <c r="E148">
-        <v>0.07854739723687533</v>
+        <v>0.079110096591472251</v>
       </c>
     </row>
     <row r="149">
@@ -3081,16 +3081,16 @@
         <v>152</v>
       </c>
       <c r="B149">
-        <v>-0.082332489561085104</v>
+        <v>-0.081867058574822155</v>
       </c>
       <c r="C149">
-        <v>0.0044269318939009232</v>
+        <v>0.004573813246563788</v>
       </c>
       <c r="D149">
-        <v>-0.091009126559884093</v>
+        <v>-0.090831578501857538</v>
       </c>
       <c r="E149">
-        <v>-0.073655852562286114</v>
+        <v>-0.072902538647786772</v>
       </c>
     </row>
     <row r="150">
@@ -3098,16 +3098,16 @@
         <v>153</v>
       </c>
       <c r="B150">
-        <v>-0.046436123814379206</v>
+        <v>-0.047965139208171012</v>
       </c>
       <c r="C150">
-        <v>0.0099229826603319284</v>
+        <v>0.011368070720195472</v>
       </c>
       <c r="D150">
-        <v>-0.065884834694186503</v>
+        <v>-0.070246174967491123</v>
       </c>
       <c r="E150">
-        <v>-0.026987412934571908</v>
+        <v>-0.025684103448850897</v>
       </c>
     </row>
     <row r="151">
@@ -3115,16 +3115,16 @@
         <v>154</v>
       </c>
       <c r="B151">
-        <v>0.030481286362379682</v>
+        <v>0.030823782799415105</v>
       </c>
       <c r="C151">
-        <v>0.0056004818220753054</v>
+        <v>0.0060420374428157425</v>
       </c>
       <c r="D151">
-        <v>0.019504531139316994</v>
+        <v>0.018981592894370791</v>
       </c>
       <c r="E151">
-        <v>0.041458041585442369</v>
+        <v>0.042665972704459418</v>
       </c>
     </row>
     <row r="152">
@@ -3132,16 +3132,16 @@
         <v>155</v>
       </c>
       <c r="B152">
-        <v>-0.14559277946367147</v>
+        <v>-0.14422467548399914</v>
       </c>
       <c r="C152">
-        <v>0.0056954447898999484</v>
+        <v>0.0052637241647830518</v>
       </c>
       <c r="D152">
-        <v>-0.15675566183515524</v>
+        <v>-0.15454140039322534</v>
       </c>
       <c r="E152">
-        <v>-0.13442989709218769</v>
+        <v>-0.13390795057477295</v>
       </c>
     </row>
     <row r="153">
@@ -3149,16 +3149,16 @@
         <v>156</v>
       </c>
       <c r="B153">
-        <v>0.0074768265195916585</v>
+        <v>0.0078061254971506329</v>
       </c>
       <c r="C153">
-        <v>0.0094828884460313612</v>
+        <v>0.010965035855227278</v>
       </c>
       <c r="D153">
-        <v>-0.011109319456693056</v>
+        <v>-0.013684981368789057</v>
       </c>
       <c r="E153">
-        <v>0.026062972495876371</v>
+        <v>0.029297232363090325</v>
       </c>
     </row>
     <row r="154">
@@ -3166,16 +3166,16 @@
         <v>157</v>
       </c>
       <c r="B154">
-        <v>0.084885942909210588</v>
+        <v>0.084370825031672605</v>
       </c>
       <c r="C154">
-        <v>0.0065850867083711061</v>
+        <v>0.0064161990827065456</v>
       </c>
       <c r="D154">
-        <v>0.071979391964862083</v>
+        <v>0.071795287479385003</v>
       </c>
       <c r="E154">
-        <v>0.097792493853559093</v>
+        <v>0.096946362583960208</v>
       </c>
     </row>
     <row r="155">
@@ -3183,16 +3183,16 @@
         <v>158</v>
       </c>
       <c r="B155">
-        <v>-0.096155394104075337</v>
+        <v>-0.095670176290849243</v>
       </c>
       <c r="C155">
-        <v>0.0052841190368163602</v>
+        <v>0.0052641782770338321</v>
       </c>
       <c r="D155">
-        <v>-0.1065120909536201</v>
+        <v>-0.10598779050681477</v>
       </c>
       <c r="E155">
-        <v>-0.08579869725453057</v>
+        <v>-0.085352562074883717</v>
       </c>
     </row>
     <row r="156">
@@ -3200,16 +3200,16 @@
         <v>159</v>
       </c>
       <c r="B156">
-        <v>-0.044488763892814684</v>
+        <v>-0.042973093175961825</v>
       </c>
       <c r="C156">
-        <v>0.010273409959815606</v>
+        <v>0.010882941841590292</v>
       </c>
       <c r="D156">
-        <v>-0.064624304334577415</v>
+        <v>-0.064303296969817181</v>
       </c>
       <c r="E156">
-        <v>-0.024353223451051949</v>
+        <v>-0.021642889382106463</v>
       </c>
     </row>
     <row r="157">
@@ -3217,16 +3217,16 @@
         <v>160</v>
       </c>
       <c r="B157">
-        <v>0.030174202803570645</v>
+        <v>0.030408090265644751</v>
       </c>
       <c r="C157">
-        <v>0.0061279745120887642</v>
+        <v>0.0065756340352743263</v>
       </c>
       <c r="D157">
-        <v>0.018163577402959333</v>
+        <v>0.0175200664125542</v>
       </c>
       <c r="E157">
-        <v>0.042184828204181957</v>
+        <v>0.043296114118735303</v>
       </c>
     </row>
     <row r="158">
@@ -3234,16 +3234,16 @@
         <v>161</v>
       </c>
       <c r="B158">
-        <v>-0.11441278129951565</v>
+        <v>-0.11333197067799086</v>
       </c>
       <c r="C158">
-        <v>0.0068132377909975632</v>
+        <v>0.0062408497525171707</v>
       </c>
       <c r="D158">
-        <v>-0.12776656958113569</v>
+        <v>-0.12556389442936028</v>
       </c>
       <c r="E158">
-        <v>-0.10105899301789563</v>
+        <v>-0.10110004692662145</v>
       </c>
     </row>
     <row r="159">
@@ -3251,16 +3251,16 @@
         <v>162</v>
       </c>
       <c r="B159">
-        <v>-0.027274438931601995</v>
+        <v>-0.031914621107633073</v>
       </c>
       <c r="C159">
-        <v>0.018647572672338082</v>
+        <v>0.020099508067918066</v>
       </c>
       <c r="D159">
-        <v>-0.063823249507618363</v>
+        <v>-0.071309200351853036</v>
       </c>
       <c r="E159">
-        <v>0.0092743716444143795</v>
+        <v>0.0074799581365868895</v>
       </c>
     </row>
     <row r="160">
@@ -3268,16 +3268,16 @@
         <v>163</v>
       </c>
       <c r="B160">
-        <v>0.042427970564149535</v>
+        <v>0.041784192322773639</v>
       </c>
       <c r="C160">
-        <v>0.01034664418098296</v>
+        <v>0.010728928783989825</v>
       </c>
       <c r="D160">
-        <v>0.022148787588815198</v>
+        <v>0.020755735618347461</v>
       </c>
       <c r="E160">
-        <v>0.062707153539483876</v>
+        <v>0.062812649027199824</v>
       </c>
     </row>
     <row r="161">
@@ -3285,16 +3285,16 @@
         <v>164</v>
       </c>
       <c r="B161">
-        <v>-0.072316157305740564</v>
+        <v>-0.072684558613459793</v>
       </c>
       <c r="C161">
-        <v>0.0071312128171248613</v>
+        <v>0.0067746692046619338</v>
       </c>
       <c r="D161">
-        <v>-0.086293189524004735</v>
+        <v>-0.085962777132474619</v>
       </c>
       <c r="E161">
-        <v>-0.058339125087476393</v>
+        <v>-0.059406340094444968</v>
       </c>
     </row>
     <row r="162">
@@ -3302,16 +3302,16 @@
         <v>165</v>
       </c>
       <c r="B162">
-        <v>-0.082582957450871256</v>
+        <v>-0.08136470327442244</v>
       </c>
       <c r="C162">
-        <v>0.02084059733832511</v>
+        <v>0.01908214413520349</v>
       </c>
       <c r="D162">
-        <v>-0.12343010476165391</v>
+        <v>-0.11876533081564761</v>
       </c>
       <c r="E162">
-        <v>-0.041735810140088606</v>
+        <v>-0.043964075733197272</v>
       </c>
     </row>
     <row r="163">
@@ -3319,16 +3319,16 @@
         <v>166</v>
       </c>
       <c r="B163">
-        <v>0.076187227073819419</v>
+        <v>0.0774392998598257</v>
       </c>
       <c r="C163">
-        <v>0.010092617063296136</v>
+        <v>0.011767487397406918</v>
       </c>
       <c r="D163">
-        <v>0.056405902707571315</v>
+        <v>0.054375255791814368</v>
       </c>
       <c r="E163">
-        <v>0.095968551440067523</v>
+        <v>0.10050334392783702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>